<commit_message>
RM-110 contracten_upload.html 80% werkend (tests working again)
</commit_message>
<xml_diff>
--- a/rm/test/resources/Overzicht_Tech_Cluster_Backend 2-12.xlsx
+++ b/rm/test/resources/Overzicht_Tech_Cluster_Backend 2-12.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t xml:space="preserve">Database nr.</t>
   </si>
@@ -127,22 +127,31 @@
     <t xml:space="preserve">Lopend contract</t>
   </si>
   <si>
-    <t xml:space="preserve">Maandelijkse Facturatie a €221,34I = geschatte éénmalige investeringskosten n.v.t.Y = aantal jaren looptijd overeenkomstX = geschatte jaarlijkse kosten</t>
+    <t xml:space="preserve">Maandelijkse Facturatie a €1000,= geschatte éénmalige investeringskosten n.v.t.Y = aantal jaren looptijd overeenkomstX = geschatte jaarlijkse kosten</t>
   </si>
   <si>
     <t xml:space="preserve">NPO/Technology/IAAS</t>
   </si>
   <si>
-    <t xml:space="preserve">Bart Adriaanse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bart.adriaanse@npo.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">035 677 8899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KRO-NCRV(AKN)-mw/0211/016 Colo remote extra 1 Gb koppeling</t>
+    <t xml:space="preserve">Eelco Aartsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eelco@aesset.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">075-6163455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pietje Puk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.puk@npo.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-1231231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneeuwbezems 2021</t>
   </si>
   <si>
     <t xml:space="preserve">Ja</t>
@@ -158,12 +167,6 @@
   </si>
   <si>
     <t xml:space="preserve">44337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eelco Aartsen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eelco@aesset.nl</t>
   </si>
 </sst>
 </file>
@@ -278,15 +281,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,7 +431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -448,13 +451,13 @@
       <c r="G2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="5" t="n">
         <v>44256.4583333333</v>
       </c>
       <c r="K2" s="3"/>
@@ -464,47 +467,47 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="5" t="n">
-        <v>2656</v>
+      <c r="R2" s="6" t="n">
+        <v>2300</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="3"/>
-      <c r="AB2" s="4" t="n">
+      <c r="AB2" s="5" t="n">
         <v>41334.4583333333</v>
       </c>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG2" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="5" t="n">
         <v>40969.4583333333</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
@@ -519,13 +522,13 @@
       <c r="G3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="5" t="n">
         <v>44256.4583333333</v>
       </c>
       <c r="K3" s="3"/>
@@ -535,47 +538,47 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="5" t="n">
-        <v>2656</v>
+      <c r="R3" s="6" t="n">
+        <v>2300</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="4" t="n">
+      <c r="AB3" s="5" t="n">
         <v>41334.4583333333</v>
       </c>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG3" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG3" s="5" t="n">
         <v>40969.4583333333</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -588,13 +591,13 @@
       <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="5" t="n">
         <v>44256.4583333333</v>
       </c>
       <c r="K4" s="3"/>
@@ -604,47 +607,47 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="5" t="n">
-        <v>2656</v>
+      <c r="R4" s="6" t="n">
+        <v>2300</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="4" t="n">
+      <c r="AB4" s="5" t="n">
         <v>41334.4583333333</v>
       </c>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG4" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG4" s="5" t="n">
         <v>40969.4583333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>34</v>
@@ -657,15 +660,15 @@
         <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="5" t="n">
         <v>44256.4583333333</v>
       </c>
       <c r="K5" s="3"/>
@@ -675,38 +678,38 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="5" t="n">
-        <v>2656</v>
+      <c r="R5" s="6" t="n">
+        <v>2300</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="4" t="n">
+      <c r="AB5" s="5" t="n">
         <v>41334.4583333333</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG5" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AG5" s="5" t="n">
         <v>40969.4583333333</v>
       </c>
     </row>
@@ -889,7 +892,14 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" display="eelco@aesset.nl"/>
+    <hyperlink ref="H2" r:id="rId1" display="eelco@aesset.nl"/>
+    <hyperlink ref="U2" r:id="rId2" display="p.puk@npo.nl"/>
+    <hyperlink ref="H3" r:id="rId3" display="eelco@aesset.nl"/>
+    <hyperlink ref="U3" r:id="rId4" display="p.puk@npo.nl"/>
+    <hyperlink ref="H4" r:id="rId5" display="eelco@aesset.nl"/>
+    <hyperlink ref="U4" r:id="rId6" display="p.puk@npo.nl"/>
+    <hyperlink ref="H5" r:id="rId7" display="eelco@aesset.nl"/>
+    <hyperlink ref="U5" r:id="rId8" display="p.puk@npo.nl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>